<commit_message>
alistamos lista de chequeo
</commit_message>
<xml_diff>
--- a/assets/Documentación/PFPL01 - Lista de chequeo producto software (1).xlsx
+++ b/assets/Documentación/PFPL01 - Lista de chequeo producto software (1).xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMBIENTE 314\Downloads\tps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\proyectoFinal\assets\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D360566-1192-4720-8E08-35EE99C63CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E47BA5-592C-460D-ACBD-9BAF16CF44EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21480" yWindow="930" windowWidth="20730" windowHeight="11760" tabRatio="772" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja de Control" sheetId="5" r:id="rId1"/>
     <sheet name="Requisitos Funcionales" sheetId="2" r:id="rId2"/>
-    <sheet name="Requisitos No Funcionales" sheetId="1" r:id="rId3"/>
-    <sheet name="Resultado" sheetId="6" r:id="rId4"/>
+    <sheet name="Requisitos Funcionales (2)" sheetId="7" r:id="rId3"/>
+    <sheet name="Requisitos No Funcionales" sheetId="1" r:id="rId4"/>
+    <sheet name="Resultado" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Hoja de Control'!$B$2:$F$39</definedName>
@@ -30,12 +31,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="135">
   <si>
     <t>Funcionalidad</t>
   </si>
@@ -82,9 +92,6 @@
     <t>Mantenibilidad</t>
   </si>
   <si>
-    <t>Nombre del Proyecto</t>
-  </si>
-  <si>
     <t>HOJA DE CONTROL</t>
   </si>
   <si>
@@ -97,16 +104,10 @@
     <t>Proyecto</t>
   </si>
   <si>
-    <t>Nombre del proyecto</t>
-  </si>
-  <si>
     <t>Entregable</t>
   </si>
   <si>
     <t>Autor</t>
-  </si>
-  <si>
-    <t>Nombre del Responsable</t>
   </si>
   <si>
     <t>Fecha Versión</t>
@@ -360,13 +361,103 @@
   </si>
   <si>
     <t>¿El sistema cuenta con facilidad para establecer criterios de prueba?</t>
+  </si>
+  <si>
+    <t>Campeche</t>
+  </si>
+  <si>
+    <t>Jose bohorquez</t>
+  </si>
+  <si>
+    <t>el sistema (Prioridad: debe [Alta], debera [MEdia], deberia,podra [Baja], permitir)</t>
+  </si>
+  <si>
+    <t>el sistema debe permitir al administrador y empleado iniciar sesion</t>
+  </si>
+  <si>
+    <t>usuarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe permitir al administrador y empleado iniciar sesión	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe permitir al administrador crear, editar y eliminar usuarios	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe permitir al usuario modificar su perfil	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe permitir al usuario ver su historial de actividad	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe permitir al usuario descargar sus datos	</t>
+  </si>
+  <si>
+    <t>No Cumple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe permitir al usuario eliminar sus datos	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe permitir al usuario invitar a amigos	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe ofrecer un programa de referidos	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario debe poder agregar un producto al carrito de compras	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario debe poder editar la cantidad de un producto en el carrito de compras	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario debe poder eliminar un producto del carrito de compras	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario debe poder pagar los productos del carrito de compras	</t>
+  </si>
+  <si>
+    <t>Carrito</t>
+  </si>
+  <si>
+    <t>productos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario debe poder buscar productos por nombre, categoría, precio o marca.	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe mostrar al usuario una lista de productos con imágenes, nombre, precio y descripción.	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe permitir al administrador agregar, editar y eliminar productos.	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario debe poder agregar un producto al carrito de compras.	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario debe poder pagar los productos del carrito de compras.	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe registrar los pedidos realizados por los usuarios.	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario debe poder ver su historial de compras.	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario debe poder calificar y reseñar los productos que ha comprado.	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe ofrecer a los usuarios recomendaciones de productos en función de su historial de compras.	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe permitir al administrador importar datos de productos desde un archivo CSV.	</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -452,6 +543,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1103,7 +1202,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1129,72 +1228,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1204,7 +1259,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1213,9 +1267,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1225,9 +1276,6 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1237,7 +1285,6 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1247,47 +1294,10 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1324,27 +1334,135 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="15" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel_BuiltIn_Hyperlink" xfId="2" xr:uid="{1EB9EC41-D830-4ACE-B66C-36C057A1DC02}"/>
@@ -1714,463 +1832,483 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A635BB-A94A-407B-BBB0-F2B3339CC475}">
   <dimension ref="A2:P82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="12" style="10" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="28" style="10" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="35.140625" style="10" customWidth="1"/>
-    <col min="7" max="8" width="12" style="10" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" style="10" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" style="10" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" style="10" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" style="10" customWidth="1"/>
-    <col min="13" max="256" width="12" style="10" customWidth="1"/>
-    <col min="257" max="257" width="12.5703125" style="10" customWidth="1"/>
-    <col min="258" max="16384" width="11.42578125" style="10"/>
+    <col min="1" max="1" width="12" style="9" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="28" style="9" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="35.140625" style="9" customWidth="1"/>
+    <col min="7" max="8" width="12" style="9" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="9" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" style="9" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" style="9" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" style="9" customWidth="1"/>
+    <col min="13" max="256" width="12" style="9" customWidth="1"/>
+    <col min="257" max="257" width="12.5703125" style="9" customWidth="1"/>
+    <col min="258" max="16384" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
     </row>
     <row r="3" spans="2:6" ht="30">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="79" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+    </row>
+    <row r="4" spans="2:6" ht="30">
+      <c r="B4" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+    </row>
+    <row r="5" spans="2:6" ht="17.25" thickBot="1">
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+    </row>
+    <row r="6" spans="2:6" ht="17.25" thickTop="1">
+      <c r="F6" s="10"/>
+    </row>
+    <row r="8" spans="2:6" ht="30">
+      <c r="B8" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-    </row>
-    <row r="4" spans="2:6" ht="30">
-      <c r="B4" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-    </row>
-    <row r="5" spans="2:6" ht="17.25" thickBot="1">
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="2:6" ht="17.25" thickTop="1">
-      <c r="F6" s="13"/>
-    </row>
-    <row r="8" spans="2:6" ht="30">
-      <c r="B8" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
     </row>
     <row r="10" spans="2:6" ht="17.25" thickBot="1"/>
     <row r="11" spans="2:6" ht="18.75" thickTop="1">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="D11" s="83"/>
+      <c r="E11" s="83"/>
+      <c r="F11" s="84"/>
+    </row>
+    <row r="12" spans="2:6" ht="18">
+      <c r="B12" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18"/>
-    </row>
-    <row r="12" spans="2:6" ht="18">
-      <c r="B12" s="19" t="s">
+      <c r="C12" s="68" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="70"/>
+    </row>
+    <row r="13" spans="2:6" ht="18.75" thickBot="1">
+      <c r="B13" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C13" s="68" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="69"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="70"/>
+    </row>
+    <row r="14" spans="2:6" ht="19.899999999999999" customHeight="1" thickTop="1">
+      <c r="B14" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="22"/>
-    </row>
-    <row r="13" spans="2:6" ht="18.75" thickBot="1">
-      <c r="B13" s="19" t="s">
+      <c r="C14" s="68" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" s="72"/>
+      <c r="E14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="22"/>
-    </row>
-    <row r="14" spans="2:6" ht="19.899999999999999" customHeight="1" thickTop="1">
-      <c r="B14" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="20" t="s">
+      <c r="F14" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="19.899999999999999" customHeight="1">
+      <c r="B15" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="25" t="s">
+      <c r="C15" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="19.899999999999999" customHeight="1">
-      <c r="B15" s="19" t="s">
+      <c r="D15" s="74"/>
+      <c r="E15" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="19.899999999999999" customHeight="1" thickBot="1">
+      <c r="B16" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C16" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="29" t="s">
+      <c r="D16" s="76"/>
+      <c r="E16" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="19.899999999999999" customHeight="1" thickBot="1">
-      <c r="B16" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="32"/>
-      <c r="E16" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="34">
+      <c r="F16" s="18">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="2:16" ht="17.25" thickTop="1">
-      <c r="B17" s="35"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="77"/>
     </row>
     <row r="18" spans="2:16" ht="19.899999999999999" customHeight="1"/>
     <row r="19" spans="2:16" ht="19.899999999999999" customHeight="1">
-      <c r="B19" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="P19" s="38" t="s">
-        <v>33</v>
+      <c r="B19" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="P19" s="21" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="19.899999999999999" customHeight="1" thickBot="1"/>
     <row r="21" spans="2:16" ht="30" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B21" s="39" t="s">
+      <c r="B21" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="66"/>
+      <c r="F21" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="40" t="s">
+    </row>
+    <row r="22" spans="2:16" ht="19.899999999999999" customHeight="1" thickTop="1">
+      <c r="B22" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="41"/>
-      <c r="F21" s="42" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" ht="19.899999999999999" customHeight="1" thickTop="1">
-      <c r="B22" s="43" t="s">
+      <c r="D22" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="45"/>
-      <c r="F22" s="46" t="s">
-        <v>25</v>
+      <c r="E22" s="67"/>
+      <c r="F22" s="27" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="2:16" ht="25.5" customHeight="1">
-      <c r="B23" s="47"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="50"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="30"/>
     </row>
     <row r="24" spans="2:16" ht="25.5" customHeight="1">
-      <c r="B24" s="47"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="50"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="30"/>
     </row>
     <row r="25" spans="2:16" ht="25.5" customHeight="1">
-      <c r="B25" s="47"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="50"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="30"/>
     </row>
     <row r="26" spans="2:16" ht="25.5" customHeight="1">
-      <c r="B26" s="47"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="50"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="30"/>
     </row>
     <row r="27" spans="2:16" ht="25.5" customHeight="1">
-      <c r="B27" s="47"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="50"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="30"/>
     </row>
     <row r="28" spans="2:16" ht="25.5" customHeight="1">
-      <c r="B28" s="47"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="50"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="30"/>
     </row>
     <row r="29" spans="2:16" ht="25.5" customHeight="1">
-      <c r="B29" s="47"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="50"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="30"/>
     </row>
     <row r="30" spans="2:16" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B30" s="51"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="54"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="33"/>
     </row>
     <row r="31" spans="2:16" ht="19.899999999999999" customHeight="1" thickTop="1"/>
     <row r="32" spans="2:16" ht="19.899999999999999" customHeight="1">
-      <c r="B32" s="37" t="s">
-        <v>39</v>
+      <c r="B32" s="20" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1" thickBot="1"/>
     <row r="34" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B34" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="56"/>
-      <c r="D34" s="56"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="57"/>
-    </row>
-    <row r="35" spans="1:13" s="58" customFormat="1" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B35" s="59"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="60"/>
-      <c r="F35" s="61"/>
-    </row>
-    <row r="36" spans="1:13" s="58" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B36" s="62"/>
-      <c r="C36" s="63"/>
-      <c r="D36" s="63"/>
-      <c r="E36" s="63"/>
-      <c r="F36" s="64"/>
-      <c r="J36" s="58" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" s="58" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B37" s="62"/>
-      <c r="C37" s="63"/>
-      <c r="D37" s="63"/>
-      <c r="E37" s="63"/>
-      <c r="F37" s="64"/>
-    </row>
-    <row r="38" spans="1:13" s="58" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B38" s="62"/>
-      <c r="C38" s="63"/>
-      <c r="D38" s="63"/>
-      <c r="E38" s="63"/>
-      <c r="F38" s="64"/>
-    </row>
-    <row r="39" spans="1:13" s="58" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B39" s="65"/>
-      <c r="C39" s="66"/>
-      <c r="D39" s="66"/>
-      <c r="E39" s="66"/>
-      <c r="F39" s="67"/>
+      <c r="B34" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="61"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="62"/>
+    </row>
+    <row r="35" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1" thickTop="1">
+      <c r="B35" s="63"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="65"/>
+    </row>
+    <row r="36" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B36" s="52"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="54"/>
+      <c r="J36" s="34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B37" s="52"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="54"/>
+    </row>
+    <row r="38" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B38" s="52"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="53"/>
+      <c r="F38" s="54"/>
+    </row>
+    <row r="39" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
+      <c r="B39" s="55"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="57"/>
     </row>
     <row r="40" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1">
-      <c r="A40" s="58"/>
-      <c r="B40" s="58"/>
+      <c r="A40" s="34"/>
+      <c r="B40" s="34"/>
     </row>
     <row r="41" spans="1:13" ht="19.899999999999999" customHeight="1">
-      <c r="A41" s="58"/>
-      <c r="B41" s="58"/>
-      <c r="C41" s="68"/>
+      <c r="A41" s="34"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="35"/>
     </row>
     <row r="42" spans="1:13" ht="19.899999999999999" customHeight="1">
-      <c r="B42" s="58"/>
+      <c r="B42" s="34"/>
     </row>
     <row r="43" spans="1:13" ht="19.899999999999999" customHeight="1">
-      <c r="A43" s="58"/>
-      <c r="B43" s="58"/>
-      <c r="K43" s="38"/>
-      <c r="L43" s="38"/>
-      <c r="M43" s="38"/>
+      <c r="A43" s="34"/>
+      <c r="B43" s="34"/>
+      <c r="K43" s="21"/>
+      <c r="L43" s="21"/>
+      <c r="M43" s="21"/>
     </row>
     <row r="44" spans="1:13" ht="19.899999999999999" customHeight="1">
-      <c r="A44" s="58"/>
-      <c r="C44" s="58"/>
-      <c r="K44" s="38"/>
-      <c r="L44" s="38"/>
-      <c r="M44" s="38"/>
+      <c r="A44" s="34"/>
+      <c r="C44" s="34"/>
+      <c r="K44" s="21"/>
+      <c r="L44" s="21"/>
+      <c r="M44" s="21"/>
     </row>
     <row r="45" spans="1:13" ht="19.899999999999999" customHeight="1">
-      <c r="A45" s="58"/>
-      <c r="B45" s="58"/>
-      <c r="C45" s="58"/>
-      <c r="K45" s="38"/>
-      <c r="L45" s="38"/>
-      <c r="M45" s="38"/>
+      <c r="A45" s="34"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="34"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="21"/>
+      <c r="M45" s="21"/>
     </row>
     <row r="46" spans="1:13" ht="19.899999999999999" customHeight="1">
-      <c r="A46" s="58"/>
-      <c r="B46" s="58"/>
-      <c r="C46" s="68"/>
-      <c r="K46" s="38"/>
-      <c r="L46" s="38"/>
-      <c r="M46" s="38"/>
+      <c r="A46" s="34"/>
+      <c r="B46" s="34"/>
+      <c r="C46" s="35"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="21"/>
     </row>
     <row r="47" spans="1:13" ht="19.899999999999999" customHeight="1">
-      <c r="A47" s="58"/>
-      <c r="B47" s="58"/>
-      <c r="K47" s="38"/>
-      <c r="L47" s="38"/>
+      <c r="A47" s="34"/>
+      <c r="B47" s="34"/>
+      <c r="K47" s="21"/>
+      <c r="L47" s="21"/>
     </row>
     <row r="48" spans="1:13" ht="19.899999999999999" customHeight="1">
-      <c r="B48" s="58"/>
-      <c r="K48" s="38"/>
-      <c r="L48" s="38"/>
+      <c r="B48" s="34"/>
+      <c r="K48" s="21"/>
+      <c r="L48" s="21"/>
     </row>
     <row r="49" spans="2:12" ht="19.899999999999999" customHeight="1">
-      <c r="B49" s="69"/>
-      <c r="K49" s="38"/>
-      <c r="L49" s="38"/>
+      <c r="B49" s="36"/>
+      <c r="K49" s="21"/>
+      <c r="L49" s="21"/>
     </row>
     <row r="50" spans="2:12" ht="19.899999999999999" customHeight="1">
-      <c r="B50" s="70"/>
-      <c r="K50" s="38"/>
-      <c r="L50" s="38"/>
+      <c r="B50" s="37"/>
+      <c r="K50" s="21"/>
+      <c r="L50" s="21"/>
     </row>
     <row r="51" spans="2:12" ht="19.899999999999999" customHeight="1">
-      <c r="F51" s="69"/>
-      <c r="K51" s="38"/>
-      <c r="L51" s="38"/>
+      <c r="F51" s="36"/>
+      <c r="K51" s="21"/>
+      <c r="L51" s="21"/>
     </row>
     <row r="52" spans="2:12" ht="19.899999999999999" customHeight="1">
-      <c r="B52" s="70"/>
-      <c r="K52" s="38"/>
-      <c r="L52" s="38"/>
+      <c r="B52" s="37"/>
+      <c r="K52" s="21"/>
+      <c r="L52" s="21"/>
     </row>
     <row r="53" spans="2:12" ht="19.899999999999999" customHeight="1">
-      <c r="F53" s="68"/>
-      <c r="K53" s="38"/>
-      <c r="L53" s="38"/>
+      <c r="F53" s="35"/>
+      <c r="K53" s="21"/>
+      <c r="L53" s="21"/>
     </row>
     <row r="54" spans="2:12" ht="19.899999999999999" customHeight="1">
-      <c r="B54" s="70"/>
-      <c r="F54" s="58"/>
-      <c r="G54" s="68"/>
-      <c r="K54" s="38"/>
-      <c r="L54" s="38"/>
+      <c r="B54" s="37"/>
+      <c r="F54" s="34"/>
+      <c r="G54" s="35"/>
+      <c r="K54" s="21"/>
+      <c r="L54" s="21"/>
     </row>
     <row r="55" spans="2:12" ht="19.899999999999999" customHeight="1">
-      <c r="F55" s="58"/>
-      <c r="G55" s="68"/>
-      <c r="K55" s="38"/>
-      <c r="L55" s="38"/>
+      <c r="F55" s="34"/>
+      <c r="G55" s="35"/>
+      <c r="K55" s="21"/>
+      <c r="L55" s="21"/>
     </row>
     <row r="56" spans="2:12" ht="19.899999999999999" customHeight="1">
-      <c r="B56" s="71"/>
-      <c r="F56" s="58"/>
-      <c r="K56" s="38"/>
-      <c r="L56" s="38"/>
+      <c r="B56" s="38"/>
+      <c r="F56" s="34"/>
+      <c r="K56" s="21"/>
+      <c r="L56" s="21"/>
     </row>
     <row r="57" spans="2:12" ht="19.899999999999999" customHeight="1">
-      <c r="F57" s="69"/>
-      <c r="K57" s="38"/>
-      <c r="L57" s="38"/>
+      <c r="F57" s="36"/>
+      <c r="K57" s="21"/>
+      <c r="L57" s="21"/>
     </row>
     <row r="58" spans="2:12" ht="19.899999999999999" customHeight="1">
-      <c r="B58" s="71"/>
-      <c r="K58" s="38"/>
-      <c r="L58" s="38"/>
+      <c r="B58" s="38"/>
+      <c r="K58" s="21"/>
+      <c r="L58" s="21"/>
     </row>
     <row r="59" spans="2:12" ht="19.899999999999999" customHeight="1">
-      <c r="K59" s="38"/>
-      <c r="L59" s="38"/>
+      <c r="K59" s="21"/>
+      <c r="L59" s="21"/>
     </row>
     <row r="60" spans="2:12" ht="19.899999999999999" customHeight="1">
-      <c r="B60" s="71"/>
+      <c r="B60" s="38"/>
     </row>
     <row r="61" spans="2:12" ht="19.899999999999999" customHeight="1"/>
     <row r="62" spans="2:12" ht="19.899999999999999" customHeight="1">
-      <c r="B62" s="71"/>
+      <c r="B62" s="38"/>
     </row>
     <row r="63" spans="2:12" ht="19.899999999999999" customHeight="1"/>
     <row r="64" spans="2:12" ht="19.899999999999999" customHeight="1">
-      <c r="B64" s="71"/>
+      <c r="B64" s="38"/>
     </row>
     <row r="65" spans="2:2" ht="19.899999999999999" customHeight="1"/>
     <row r="66" spans="2:2" ht="19.899999999999999" customHeight="1">
-      <c r="B66" s="71"/>
+      <c r="B66" s="38"/>
     </row>
     <row r="67" spans="2:2" ht="19.899999999999999" customHeight="1"/>
     <row r="68" spans="2:2" ht="19.899999999999999" customHeight="1">
-      <c r="B68" s="71"/>
+      <c r="B68" s="38"/>
     </row>
     <row r="69" spans="2:2" ht="19.899999999999999" customHeight="1"/>
     <row r="70" spans="2:2" ht="19.899999999999999" customHeight="1">
-      <c r="B70" s="71"/>
+      <c r="B70" s="38"/>
     </row>
     <row r="71" spans="2:2" ht="19.899999999999999" customHeight="1"/>
     <row r="72" spans="2:2" ht="19.899999999999999" customHeight="1">
-      <c r="B72" s="71"/>
+      <c r="B72" s="38"/>
     </row>
     <row r="73" spans="2:2" ht="19.899999999999999" customHeight="1"/>
     <row r="74" spans="2:2">
-      <c r="B74" s="71"/>
+      <c r="B74" s="38"/>
     </row>
     <row r="76" spans="2:2">
-      <c r="B76" s="71"/>
+      <c r="B76" s="38"/>
     </row>
     <row r="78" spans="2:2">
-      <c r="B78" s="71"/>
+      <c r="B78" s="38"/>
     </row>
     <row r="80" spans="2:2">
-      <c r="B80" s="71"/>
+      <c r="B80" s="38"/>
     </row>
     <row r="81" spans="2:3">
-      <c r="B81" s="68"/>
+      <c r="B81" s="35"/>
     </row>
     <row r="82" spans="2:3">
-      <c r="C82" s="68"/>
+      <c r="C82" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
     <mergeCell ref="B36:F36"/>
     <mergeCell ref="B37:F37"/>
     <mergeCell ref="B38:F38"/>
@@ -2181,24 +2319,6 @@
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="B34:F34"/>
     <mergeCell ref="B35:F35"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="C11:F11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
@@ -2211,35 +2331,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EC27DB5-F54D-4E92-8170-7A53853F8C0C}">
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="70.7109375" customWidth="1"/>
+    <col min="2" max="2" width="75.140625" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="70.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A1" s="77" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="75"/>
+      <c r="A1" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="41"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="72" t="s">
+      <c r="C2" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="72" t="s">
+      <c r="D2" s="39" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2247,7 +2371,9 @@
       <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="C3" s="5"/>
       <c r="D3" s="6" t="str">
         <f>IF(C3="Cumple","Ninguna","")</f>
@@ -2258,7 +2384,9 @@
       <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="6" t="s">
+        <v>108</v>
+      </c>
       <c r="C4" s="5"/>
       <c r="D4" s="6" t="str">
         <f t="shared" ref="D4:D17" si="0">IF(C4="Cumple","Ninguna","")</f>
@@ -2409,24 +2537,24 @@
       </c>
     </row>
     <row r="18" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="77" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="76"/>
-      <c r="C18" s="74"/>
-      <c r="D18" s="75"/>
+      <c r="A18" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="43"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="42"/>
     </row>
     <row r="19" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="78" t="s">
+      <c r="A19" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="72" t="s">
+      <c r="B19" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="72" t="s">
+      <c r="C19" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="72" t="s">
+      <c r="D19" s="39" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2596,24 +2724,24 @@
       </c>
     </row>
     <row r="35" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A35" s="77" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" s="76"/>
-      <c r="C35" s="74"/>
-      <c r="D35" s="75"/>
+      <c r="A35" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="43"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="42"/>
     </row>
     <row r="36" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A36" s="78" t="s">
+      <c r="A36" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="72" t="s">
+      <c r="B36" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="72" t="s">
+      <c r="C36" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="72" t="s">
+      <c r="D36" s="39" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2783,24 +2911,24 @@
       </c>
     </row>
     <row r="52" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A52" s="77" t="s">
-        <v>49</v>
-      </c>
-      <c r="B52" s="76"/>
-      <c r="C52" s="74"/>
-      <c r="D52" s="75"/>
+      <c r="A52" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52" s="43"/>
+      <c r="C52" s="41"/>
+      <c r="D52" s="42"/>
     </row>
     <row r="53" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A53" s="78" t="s">
+      <c r="A53" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B53" s="72" t="s">
+      <c r="B53" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="72" t="s">
+      <c r="C53" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="72" t="s">
+      <c r="D53" s="39" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2970,24 +3098,24 @@
       </c>
     </row>
     <row r="69" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A69" s="77" t="s">
-        <v>53</v>
-      </c>
-      <c r="B69" s="76"/>
-      <c r="C69" s="74"/>
-      <c r="D69" s="75"/>
+      <c r="A69" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="B69" s="43"/>
+      <c r="C69" s="41"/>
+      <c r="D69" s="42"/>
     </row>
     <row r="70" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A70" s="78" t="s">
+      <c r="A70" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B70" s="72" t="s">
+      <c r="B70" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="72" t="s">
+      <c r="C70" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D70" s="72" t="s">
+      <c r="D70" s="39" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3002,30 +3130,911 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E8C143B-B431-458E-8866-1207E50001AB}">
+  <dimension ref="A1:D70"/>
+  <sheetViews>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.42578125" style="90" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77.5703125" style="90" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
+      <c r="A1" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="91" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="41"/>
+      <c r="D1" s="88"/>
+    </row>
+    <row r="2" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A2" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="89" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="87" t="str">
+        <f>IF(C3="Cumple","Ninguna"," - El sistema debe autenticar al usuario mediante un nombre de usuario y contraseña. - El sistema debe permitir al usuario restablecer su contraseña en caso de olvido ")</f>
+        <v xml:space="preserve"> - El sistema debe autenticar al usuario mediante un nombre de usuario y contraseña. - El sistema debe permitir al usuario restablecer su contraseña en caso de olvido </v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A4" s="8">
+        <v>2</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="50" t="str">
+        <f>IF(C4="Cumple","Ninguna","- El administrador debe poder crear nuevos usuarios con diferentes roles y permisos. - El administrador debe poder editar la información de los usuarios existentes. - El administrador debe poder eliminar usuarios que ya no sean necesarios")</f>
+        <v>- El administrador debe poder crear nuevos usuarios con diferentes roles y permisos. - El administrador debe poder editar la información de los usuarios existentes. - El administrador debe poder eliminar usuarios que ya no sean necesarios</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="50" t="str">
+        <f>IF(C5="Cumple","Ninguna","- El usuario debe poder modificar su nombre, correo electrónico y contraseña. - El usuario debe poder subir una foto de perfil")</f>
+        <v>- El usuario debe poder modificar su nombre, correo electrónico y contraseña. - El usuario debe poder subir una foto de perfil</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A6" s="8">
+        <v>4</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="50" t="str">
+        <f>IF(C6="Cumple","Ninguna","- El usuario debe poder ver las acciones que ha realizado en el sistema. - El historial de actividad debe incluir la fecha, hora, acción realizada y el módulo afectado")</f>
+        <v>- El usuario debe poder ver las acciones que ha realizado en el sistema. - El historial de actividad debe incluir la fecha, hora, acción realizada y el módulo afectado</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A7" s="8">
+        <v>5</v>
+      </c>
+      <c r="B7" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="50" t="str">
+        <f>IF(C7="Cumple","Ninguna","- El usuario debe poder descargar una copia de sus datos personales en un formato legible. - Los datos descargados deben incluir el nombre, correo electrónico, foto de perfil, historial de actividad y cualquier otra información personal del usuario")</f>
+        <v>- El usuario debe poder descargar una copia de sus datos personales en un formato legible. - Los datos descargados deben incluir el nombre, correo electrónico, foto de perfil, historial de actividad y cualquier otra información personal del usuario</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A8" s="8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="50" t="str">
+        <f>IF(C8="Cumple","Ninguna","- El usuario debe poder eliminar sus datos personales de forma permanente. - El sistema debe solicitar al usuario confirmación antes de eliminar sus datos")</f>
+        <v>- El usuario debe poder eliminar sus datos personales de forma permanente. - El sistema debe solicitar al usuario confirmación antes de eliminar sus datos</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A9" s="8">
+        <v>7</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="50" t="str">
+        <f>IF(C9="Cumple","Ninguna","- El usuario debe poder enviar invitaciones a amigos por correo electrónico o a través de redes sociales. - Las invitaciones deben incluir un enlace para que los amigos puedan registrarse en el sistema")</f>
+        <v>- El usuario debe poder enviar invitaciones a amigos por correo electrónico o a través de redes sociales. - Las invitaciones deben incluir un enlace para que los amigos puedan registrarse en el sistema</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A10" s="8">
+        <v>8</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="50" t="str">
+        <f>IF(C10="Cumple","Ninguna","- El usuario debe poder ganar puntos o beneficios por referir amigos al sistema. - El sistema debe mostrar al usuario el número de amigos que ha referido y los puntos o beneficios que ha ganado")</f>
+        <v>- El usuario debe poder ganar puntos o beneficios por referir amigos al sistema. - El sistema debe mostrar al usuario el número de amigos que ha referido y los puntos o beneficios que ha ganado</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A11" s="8">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A12" s="8">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A13" s="8">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A14" s="8">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A15" s="8">
+        <v>13</v>
+      </c>
+      <c r="B15" s="50"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="50" t="str">
+        <f t="shared" ref="D4:D17" si="0">IF(C15="Cumple","Ninguna","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A16" s="8">
+        <v>14</v>
+      </c>
+      <c r="B16" s="50"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="50" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A17" s="8">
+        <v>15</v>
+      </c>
+      <c r="B17" s="50"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="50" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
+      <c r="A18" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="91" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" s="41"/>
+      <c r="D18" s="88"/>
+    </row>
+    <row r="19" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A19" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="89" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A20" s="8">
+        <v>16</v>
+      </c>
+      <c r="B20" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D20" s="50" t="str">
+        <f>IF(C20="Cumple","Ninguna","- El usuario debe poder seleccionar un producto y la cantidad deseada. - El sistema debe mostrar al usuario el precio total del producto, incluyendo impuestos y envío")</f>
+        <v>- El usuario debe poder seleccionar un producto y la cantidad deseada. - El sistema debe mostrar al usuario el precio total del producto, incluyendo impuestos y envío</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A21" s="8">
+        <v>17</v>
+      </c>
+      <c r="B21" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21" s="50" t="str">
+        <f>IF(C21="Cumple","Ninguna","- El usuario debe poder aumentar o disminuir la cantidad de un producto en el carrito de compras. - El sistema debe actualizar automáticamente el precio total del producto")</f>
+        <v>- El usuario debe poder aumentar o disminuir la cantidad de un producto en el carrito de compras. - El sistema debe actualizar automáticamente el precio total del producto</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A22" s="8">
+        <v>18</v>
+      </c>
+      <c r="B22" s="50" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" s="50" t="str">
+        <f>IF(C22="Cumple","Ninguna","- El usuario debe poder eliminar un producto del carrito de compras. - El sistema debe actualizar automáticamente el precio total del carrito de compras")</f>
+        <v>- El usuario debe poder eliminar un producto del carrito de compras. - El sistema debe actualizar automáticamente el precio total del carrito de compras</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A23" s="8">
+        <v>19</v>
+      </c>
+      <c r="B23" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" s="50" t="str">
+        <f>IF(C23="Cumple","Ninguna","- El usuario debe poder seleccionar un método de pago, como tarjeta de crédito, débito o PayPal. - El sistema debe procesar el pago de forma segura y enviar un correo electrónico de confirmación al usuario")</f>
+        <v>- El usuario debe poder seleccionar un método de pago, como tarjeta de crédito, débito o PayPal. - El sistema debe procesar el pago de forma segura y enviar un correo electrónico de confirmación al usuario</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A24" s="8">
+        <v>20</v>
+      </c>
+      <c r="B24" s="50"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="50" t="str">
+        <f t="shared" ref="D20:D34" si="1">IF(C24="Cumple","Ninguna","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A25" s="8">
+        <v>21</v>
+      </c>
+      <c r="B25" s="50"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A26" s="8">
+        <v>22</v>
+      </c>
+      <c r="B26" s="50"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A27" s="8">
+        <v>23</v>
+      </c>
+      <c r="B27" s="50"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A28" s="8">
+        <v>24</v>
+      </c>
+      <c r="B28" s="50"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A29" s="8">
+        <v>25</v>
+      </c>
+      <c r="B29" s="50"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A30" s="8">
+        <v>26</v>
+      </c>
+      <c r="B30" s="50"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A31" s="8">
+        <v>27</v>
+      </c>
+      <c r="B31" s="50"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A32" s="8">
+        <v>28</v>
+      </c>
+      <c r="B32" s="50"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A33" s="8">
+        <v>29</v>
+      </c>
+      <c r="B33" s="50"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A34" s="8">
+        <v>30</v>
+      </c>
+      <c r="B34" s="50"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
+      <c r="A35" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="91" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" s="41"/>
+      <c r="D35" s="88"/>
+    </row>
+    <row r="36" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A36" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="89" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A37" s="8">
+        <v>31</v>
+      </c>
+      <c r="B37" s="50" t="s">
+        <v>125</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D37" s="50" t="str">
+        <f>IF(C37="Cumple","Ninguna","- El sistema debe mostrar al usuario una lista de productos con imágenes, nombre, precio y descripción")</f>
+        <v>- El sistema debe mostrar al usuario una lista de productos con imágenes, nombre, precio y descripción</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A38" s="8">
+        <v>32</v>
+      </c>
+      <c r="B38" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D38" s="50" t="str">
+        <f>IF(C38="Cumple","Ninguna","- El usuario debe poder ver los detalles de un producto específico, incluyendo imágenes, descripción, precio, disponibilidad, características y especificaciones")</f>
+        <v>- El usuario debe poder ver los detalles de un producto específico, incluyendo imágenes, descripción, precio, disponibilidad, características y especificaciones</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A39" s="8">
+        <v>33</v>
+      </c>
+      <c r="B39" s="50" t="s">
+        <v>127</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D39" s="50" t="str">
+        <f>IF(C39="Cumple","Ninguna","- El administrador debe poder establecer el precio, la disponibilidad, las características y las especificaciones de un producto. - El administrador debe poder subir imágenes del producto")</f>
+        <v>- El administrador debe poder establecer el precio, la disponibilidad, las características y las especificaciones de un producto. - El administrador debe poder subir imágenes del producto</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A40" s="8">
+        <v>34</v>
+      </c>
+      <c r="B40" s="50" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40" s="50" t="str">
+        <f>IF(C40="Cumple","Ninguna","- El usuario debe poder editar la cantidad de un producto en el carrito de compras. - El usuario debe poder eliminar un producto del carrito de compras")</f>
+        <v>- El usuario debe poder editar la cantidad de un producto en el carrito de compras. - El usuario debe poder eliminar un producto del carrito de compras</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A41" s="8">
+        <v>35</v>
+      </c>
+      <c r="B41" s="50" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D41" s="50" t="str">
+        <f>IF(C41="Cumple","Ninguna","- El sistema debe aceptar diferentes métodos de pago, como tarjeta de crédito, débito o PayPal. - El sistema debe procesar el pago de forma segura y enviar un correo electrónico de confirmación al usuario")</f>
+        <v>- El sistema debe aceptar diferentes métodos de pago, como tarjeta de crédito, débito o PayPal. - El sistema debe procesar el pago de forma segura y enviar un correo electrónico de confirmación al usuario</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A42" s="8">
+        <v>36</v>
+      </c>
+      <c r="B42" s="50" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" s="50" t="str">
+        <f>IF(C42="Cumple","Ninguna","- El usuario debe poder ver el estado de su pedido. - El sistema debe enviar un correo electrónico de confirmación al usuario cuando se envíe su pedido")</f>
+        <v>- El usuario debe poder ver el estado de su pedido. - El sistema debe enviar un correo electrónico de confirmación al usuario cuando se envíe su pedido</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A43" s="8">
+        <v>37</v>
+      </c>
+      <c r="B43" s="50" t="s">
+        <v>131</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D43" s="50" t="str">
+        <f>IF(C43="Cumple","Ninguna","- El usuario debe poder ver los detalles de cada compra, como la fecha, el número de pedido, los productos comprados y el precio total")</f>
+        <v>- El usuario debe poder ver los detalles de cada compra, como la fecha, el número de pedido, los productos comprados y el precio total</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A44" s="8">
+        <v>38</v>
+      </c>
+      <c r="B44" s="50" t="s">
+        <v>132</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D44" s="50" t="str">
+        <f>IF(C44="Cumple","Ninguna","- El sistema debe mostrar las calificaciones y reseñas de los productos a otros usuarios")</f>
+        <v>- El sistema debe mostrar las calificaciones y reseñas de los productos a otros usuarios</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A45" s="8">
+        <v>39</v>
+      </c>
+      <c r="B45" s="50" t="s">
+        <v>133</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D45" s="50" t="str">
+        <f>IF(C45="Cumple","Ninguna","- El sistema debe mantener un registro del inventario de productos. - El sistema debe alertar al administrador cuando el inventario de un producto esté bajo")</f>
+        <v>- El sistema debe mantener un registro del inventario de productos. - El sistema debe alertar al administrador cuando el inventario de un producto esté bajo</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A46" s="8">
+        <v>40</v>
+      </c>
+      <c r="B46" s="50" t="s">
+        <v>134</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D46" s="50" t="str">
+        <f>IF(C46="Cumple","Ninguna","- El sistema debe permitir al administrador exportar datos de productos a un archivo CSV")</f>
+        <v>- El sistema debe permitir al administrador exportar datos de productos a un archivo CSV</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A47" s="8">
+        <v>41</v>
+      </c>
+      <c r="B47" s="50"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="50" t="str">
+        <f t="shared" ref="D37:D51" si="2">IF(C47="Cumple","Ninguna","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A48" s="8">
+        <v>42</v>
+      </c>
+      <c r="B48" s="50"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="50" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A49" s="8">
+        <v>43</v>
+      </c>
+      <c r="B49" s="50"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="50" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A50" s="8">
+        <v>44</v>
+      </c>
+      <c r="B50" s="50"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="50" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A51" s="8">
+        <v>45</v>
+      </c>
+      <c r="B51" s="50"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="50" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
+      <c r="A52" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52" s="91"/>
+      <c r="C52" s="41"/>
+      <c r="D52" s="88"/>
+    </row>
+    <row r="53" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A53" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="89" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A54" s="8">
+        <v>46</v>
+      </c>
+      <c r="B54" s="50"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="50" t="str">
+        <f t="shared" ref="D54:D68" si="3">IF(C54="Cumple","Ninguna","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A55" s="8">
+        <v>47</v>
+      </c>
+      <c r="B55" s="50"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="50" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A56" s="8">
+        <v>48</v>
+      </c>
+      <c r="B56" s="50"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="50" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A57" s="8">
+        <v>49</v>
+      </c>
+      <c r="B57" s="50"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="50" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A58" s="8">
+        <v>50</v>
+      </c>
+      <c r="B58" s="50"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="50" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A59" s="8">
+        <v>51</v>
+      </c>
+      <c r="B59" s="50"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="50" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A60" s="8">
+        <v>52</v>
+      </c>
+      <c r="B60" s="50"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="50" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A61" s="8">
+        <v>53</v>
+      </c>
+      <c r="B61" s="50"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="50" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A62" s="8">
+        <v>54</v>
+      </c>
+      <c r="B62" s="50"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="50" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A63" s="8">
+        <v>55</v>
+      </c>
+      <c r="B63" s="50"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="50" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A64" s="8">
+        <v>56</v>
+      </c>
+      <c r="B64" s="50"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="50" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A65" s="8">
+        <v>57</v>
+      </c>
+      <c r="B65" s="50"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="50" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A66" s="8">
+        <v>58</v>
+      </c>
+      <c r="B66" s="50"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="50" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A67" s="8">
+        <v>59</v>
+      </c>
+      <c r="B67" s="50"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="50" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A68" s="8">
+        <v>60</v>
+      </c>
+      <c r="B68" s="50"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="50" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
+      <c r="A69" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="B69" s="91"/>
+      <c r="C69" s="41"/>
+      <c r="D69" s="88"/>
+    </row>
+    <row r="70" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A70" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B70" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" s="89" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C37:C51 C54:C68 C20:C34 C3:C10 C15:C17" xr:uid="{82A3AD37-52EC-47BB-B888-C5A1A9C7F077}">
+      <formula1>"Cumple, No Cumple"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="90.7109375" style="86" customWidth="1"/>
+    <col min="2" max="2" width="90.7109375" style="51" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="70.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="39" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3033,10 +4042,12 @@
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="92" t="s">
+        <v>115</v>
+      </c>
       <c r="D2" s="6" t="str">
         <f>IF(C2="Cumple","Ninguna","")</f>
         <v/>
@@ -3046,10 +4057,12 @@
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D3" s="6" t="str">
         <f t="shared" ref="D3:D65" si="0">IF(C3="Cumple","Ninguna","")</f>
         <v/>
@@ -3059,10 +4072,12 @@
       <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3072,10 +4087,12 @@
       <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="85" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="5"/>
+      <c r="B5" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3085,10 +4102,12 @@
       <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="85" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="5"/>
+      <c r="B6" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3098,10 +4117,12 @@
       <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="85" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="5"/>
+      <c r="B7" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3111,10 +4132,12 @@
       <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="85" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="5"/>
+      <c r="B8" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3124,26 +4147,28 @@
       <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" s="85" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="5"/>
+      <c r="B9" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A10" s="72" t="s">
+      <c r="A10" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="72" t="s">
+      <c r="D10" s="39" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3151,10 +4176,12 @@
       <c r="A11" s="8">
         <v>9</v>
       </c>
-      <c r="B11" s="85" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="5"/>
+      <c r="B11" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3164,10 +4191,12 @@
       <c r="A12" s="8">
         <v>10</v>
       </c>
-      <c r="B12" s="85" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="5"/>
+      <c r="B12" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3177,10 +4206,12 @@
       <c r="A13" s="8">
         <v>11</v>
       </c>
-      <c r="B13" s="85" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="5"/>
+      <c r="B13" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3190,10 +4221,12 @@
       <c r="A14" s="8">
         <v>12</v>
       </c>
-      <c r="B14" s="85" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="5"/>
+      <c r="B14" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3203,10 +4236,12 @@
       <c r="A15" s="8">
         <v>13</v>
       </c>
-      <c r="B15" s="85" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" s="5"/>
+      <c r="B15" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3216,10 +4251,12 @@
       <c r="A16" s="8">
         <v>14</v>
       </c>
-      <c r="B16" s="85" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="5"/>
+      <c r="B16" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3229,26 +4266,28 @@
       <c r="A17" s="8">
         <v>15</v>
       </c>
-      <c r="B17" s="85" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="5"/>
+      <c r="B17" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="72" t="s">
+      <c r="A18" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="72" t="s">
+      <c r="C18" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="72" t="s">
+      <c r="D18" s="39" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3256,10 +4295,12 @@
       <c r="A19" s="8">
         <v>16</v>
       </c>
-      <c r="B19" s="85" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="5"/>
+      <c r="B19" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3269,10 +4310,12 @@
       <c r="A20" s="8">
         <v>17</v>
       </c>
-      <c r="B20" s="85" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="5"/>
+      <c r="B20" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3282,10 +4325,12 @@
       <c r="A21" s="8">
         <v>18</v>
       </c>
-      <c r="B21" s="85" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" s="5"/>
+      <c r="B21" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3295,10 +4340,12 @@
       <c r="A22" s="8">
         <v>19</v>
       </c>
-      <c r="B22" s="85" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="5"/>
+      <c r="B22" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3308,10 +4355,12 @@
       <c r="A23" s="8">
         <v>20</v>
       </c>
-      <c r="B23" s="85" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="5"/>
+      <c r="B23" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3321,10 +4370,12 @@
       <c r="A24" s="8">
         <v>21</v>
       </c>
-      <c r="B24" s="85" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="5"/>
+      <c r="B24" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3334,10 +4385,12 @@
       <c r="A25" s="8">
         <v>22</v>
       </c>
-      <c r="B25" s="85" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" s="5"/>
+      <c r="B25" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3347,26 +4400,28 @@
       <c r="A26" s="8">
         <v>23</v>
       </c>
-      <c r="B26" s="85" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="5"/>
+      <c r="B26" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="27" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A27" s="72" t="s">
+      <c r="A27" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="72" t="s">
+      <c r="B27" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="72" t="s">
+      <c r="C27" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="72" t="s">
+      <c r="D27" s="39" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3374,10 +4429,12 @@
       <c r="A28" s="8">
         <v>24</v>
       </c>
-      <c r="B28" s="85" t="s">
-        <v>74</v>
-      </c>
-      <c r="C28" s="5"/>
+      <c r="B28" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3387,10 +4444,12 @@
       <c r="A29" s="8">
         <v>25</v>
       </c>
-      <c r="B29" s="85" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" s="5"/>
+      <c r="B29" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3400,10 +4459,12 @@
       <c r="A30" s="8">
         <v>26</v>
       </c>
-      <c r="B30" s="85" t="s">
-        <v>76</v>
-      </c>
-      <c r="C30" s="5"/>
+      <c r="B30" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3413,10 +4474,12 @@
       <c r="A31" s="8">
         <v>27</v>
       </c>
-      <c r="B31" s="85" t="s">
-        <v>77</v>
-      </c>
-      <c r="C31" s="5"/>
+      <c r="B31" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3426,10 +4489,12 @@
       <c r="A32" s="8">
         <v>28</v>
       </c>
-      <c r="B32" s="85" t="s">
-        <v>78</v>
-      </c>
-      <c r="C32" s="5"/>
+      <c r="B32" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3439,26 +4504,28 @@
       <c r="A33" s="8">
         <v>29</v>
       </c>
-      <c r="B33" s="85" t="s">
-        <v>79</v>
-      </c>
-      <c r="C33" s="5"/>
+      <c r="B33" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D33" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="34" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A34" s="72" t="s">
+      <c r="A34" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="72" t="s">
+      <c r="C34" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="72" t="s">
+      <c r="D34" s="39" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3466,10 +4533,12 @@
       <c r="A35" s="8">
         <v>30</v>
       </c>
-      <c r="B35" s="85" t="s">
-        <v>80</v>
-      </c>
-      <c r="C35" s="5"/>
+      <c r="B35" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3479,10 +4548,12 @@
       <c r="A36" s="8">
         <v>31</v>
       </c>
-      <c r="B36" s="85" t="s">
-        <v>81</v>
-      </c>
-      <c r="C36" s="5"/>
+      <c r="B36" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3492,26 +4563,28 @@
       <c r="A37" s="8">
         <v>32</v>
       </c>
-      <c r="B37" s="85" t="s">
-        <v>82</v>
-      </c>
-      <c r="C37" s="5"/>
+      <c r="B37" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="38" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A38" s="72" t="s">
+      <c r="A38" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="72" t="s">
+      <c r="B38" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="72" t="s">
+      <c r="C38" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="72" t="s">
+      <c r="D38" s="39" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3519,10 +4592,12 @@
       <c r="A39" s="8">
         <v>33</v>
       </c>
-      <c r="B39" s="85" t="s">
-        <v>83</v>
-      </c>
-      <c r="C39" s="5"/>
+      <c r="B39" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3532,10 +4607,12 @@
       <c r="A40" s="8">
         <v>34</v>
       </c>
-      <c r="B40" s="85" t="s">
-        <v>84</v>
-      </c>
-      <c r="C40" s="5"/>
+      <c r="B40" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3545,10 +4622,12 @@
       <c r="A41" s="8">
         <v>35</v>
       </c>
-      <c r="B41" s="85" t="s">
-        <v>85</v>
-      </c>
-      <c r="C41" s="5"/>
+      <c r="B41" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D41" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3558,10 +4637,12 @@
       <c r="A42" s="8">
         <v>36</v>
       </c>
-      <c r="B42" s="85" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" s="5"/>
+      <c r="B42" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D42" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3571,10 +4652,12 @@
       <c r="A43" s="8">
         <v>37</v>
       </c>
-      <c r="B43" s="85" t="s">
-        <v>87</v>
-      </c>
-      <c r="C43" s="5"/>
+      <c r="B43" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D43" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3584,10 +4667,12 @@
       <c r="A44" s="8">
         <v>38</v>
       </c>
-      <c r="B44" s="85" t="s">
-        <v>88</v>
-      </c>
-      <c r="C44" s="5"/>
+      <c r="B44" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D44" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3597,10 +4682,12 @@
       <c r="A45" s="8">
         <v>39</v>
       </c>
-      <c r="B45" s="85" t="s">
-        <v>89</v>
-      </c>
-      <c r="C45" s="5"/>
+      <c r="B45" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D45" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3610,10 +4697,12 @@
       <c r="A46" s="8">
         <v>40</v>
       </c>
-      <c r="B46" s="85" t="s">
-        <v>90</v>
-      </c>
-      <c r="C46" s="5"/>
+      <c r="B46" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D46" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3623,10 +4712,12 @@
       <c r="A47" s="8">
         <v>41</v>
       </c>
-      <c r="B47" s="85" t="s">
-        <v>91</v>
-      </c>
-      <c r="C47" s="5"/>
+      <c r="B47" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D47" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3636,26 +4727,28 @@
       <c r="A48" s="8">
         <v>42</v>
       </c>
-      <c r="B48" s="85" t="s">
-        <v>92</v>
-      </c>
-      <c r="C48" s="5"/>
+      <c r="B48" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D48" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="49" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A49" s="72" t="s">
+      <c r="A49" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="72" t="s">
+      <c r="B49" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C49" s="72" t="s">
+      <c r="C49" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D49" s="72" t="s">
+      <c r="D49" s="39" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3663,10 +4756,12 @@
       <c r="A50" s="8">
         <v>43</v>
       </c>
-      <c r="B50" s="85" t="s">
-        <v>93</v>
-      </c>
-      <c r="C50" s="5"/>
+      <c r="B50" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D50" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3676,10 +4771,12 @@
       <c r="A51" s="8">
         <v>44</v>
       </c>
-      <c r="B51" s="85" t="s">
-        <v>94</v>
-      </c>
-      <c r="C51" s="5"/>
+      <c r="B51" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D51" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3689,10 +4786,12 @@
       <c r="A52" s="8">
         <v>45</v>
       </c>
-      <c r="B52" s="85" t="s">
-        <v>95</v>
-      </c>
-      <c r="C52" s="5"/>
+      <c r="B52" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D52" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3702,10 +4801,12 @@
       <c r="A53" s="8">
         <v>46</v>
       </c>
-      <c r="B53" s="85" t="s">
-        <v>96</v>
-      </c>
-      <c r="C53" s="5"/>
+      <c r="B53" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D53" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3715,10 +4816,12 @@
       <c r="A54" s="8">
         <v>47</v>
       </c>
-      <c r="B54" s="85" t="s">
-        <v>97</v>
-      </c>
-      <c r="C54" s="5"/>
+      <c r="B54" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D54" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3728,10 +4831,12 @@
       <c r="A55" s="8">
         <v>48</v>
       </c>
-      <c r="B55" s="85" t="s">
-        <v>98</v>
-      </c>
-      <c r="C55" s="5"/>
+      <c r="B55" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D55" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3741,10 +4846,12 @@
       <c r="A56" s="8">
         <v>49</v>
       </c>
-      <c r="B56" s="85" t="s">
-        <v>99</v>
-      </c>
-      <c r="C56" s="5"/>
+      <c r="B56" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D56" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3754,10 +4861,12 @@
       <c r="A57" s="8">
         <v>50</v>
       </c>
-      <c r="B57" s="85" t="s">
-        <v>100</v>
-      </c>
-      <c r="C57" s="5"/>
+      <c r="B57" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D57" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3767,10 +4876,12 @@
       <c r="A58" s="8">
         <v>51</v>
       </c>
-      <c r="B58" s="85" t="s">
-        <v>101</v>
-      </c>
-      <c r="C58" s="5"/>
+      <c r="B58" s="50" t="s">
+        <v>98</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D58" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3780,26 +4891,28 @@
       <c r="A59" s="8">
         <v>52</v>
       </c>
-      <c r="B59" s="85" t="s">
-        <v>102</v>
-      </c>
-      <c r="C59" s="5"/>
+      <c r="B59" s="50" t="s">
+        <v>99</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D59" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="60" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A60" s="72" t="s">
+      <c r="A60" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B60" s="72" t="s">
+      <c r="B60" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="C60" s="72" t="s">
+      <c r="C60" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D60" s="72" t="s">
+      <c r="D60" s="39" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3807,10 +4920,12 @@
       <c r="A61" s="8">
         <v>53</v>
       </c>
-      <c r="B61" s="85" t="s">
-        <v>103</v>
-      </c>
-      <c r="C61" s="5"/>
+      <c r="B61" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D61" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3820,10 +4935,12 @@
       <c r="A62" s="8">
         <v>54</v>
       </c>
-      <c r="B62" s="85" t="s">
-        <v>104</v>
-      </c>
-      <c r="C62" s="5"/>
+      <c r="B62" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D62" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3833,10 +4950,12 @@
       <c r="A63" s="8">
         <v>55</v>
       </c>
-      <c r="B63" s="85" t="s">
-        <v>105</v>
-      </c>
-      <c r="C63" s="5"/>
+      <c r="B63" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D63" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3846,10 +4965,12 @@
       <c r="A64" s="8">
         <v>56</v>
       </c>
-      <c r="B64" s="85" t="s">
-        <v>106</v>
-      </c>
-      <c r="C64" s="5"/>
+      <c r="B64" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D64" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3859,10 +4980,12 @@
       <c r="A65" s="8">
         <v>57</v>
       </c>
-      <c r="B65" s="85" t="s">
-        <v>107</v>
-      </c>
-      <c r="C65" s="5"/>
+      <c r="B65" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D65" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3870,7 +4993,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C9 C11:C17 C19:C26 C28:C32 C50:C59 C39:C48 C33 C35:C37" xr:uid="{28946FFD-2DE3-4AFF-8B02-311FA9F788A5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C9 C28:C33 C11:C17 C39:C48 C35:C37 C19:C26 C50:C59 C61:C65" xr:uid="{28946FFD-2DE3-4AFF-8B02-311FA9F788A5}">
       <formula1>"Cumple, No Cumple"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3878,46 +5001,48 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D51D51-DE4C-4B5C-90F6-8EADB68EB458}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView zoomScale="230" zoomScaleNormal="230" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="73" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="85" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="4" customFormat="1">
+      <c r="A2" s="47">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>44</v>
-      </c>
-      <c r="B1" s="79" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="79" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="79" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="79" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="81" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="4" customFormat="1">
-      <c r="A2" s="82">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="C2" s="5">
         <f>COUNT('Requisitos Funcionales'!A:A)</f>
@@ -3927,18 +5052,18 @@
         <f>COUNTIF('Requisitos Funcionales'!C2:C68,"Cumple")</f>
         <v>0</v>
       </c>
-      <c r="E2" s="83">
+      <c r="E2" s="48">
         <f>D2/C2%</f>
         <v>0</v>
       </c>
-      <c r="F2" s="80"/>
+      <c r="F2" s="86"/>
     </row>
     <row r="3" spans="1:6" s="4" customFormat="1">
-      <c r="A3" s="82">
+      <c r="A3" s="47">
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C3" s="5">
         <f>COUNT('Requisitos No Funcionales'!A:A)</f>
@@ -3948,22 +5073,22 @@
         <f>COUNTIF('Requisitos No Funcionales'!C:C,"Cumple")</f>
         <v>0</v>
       </c>
-      <c r="E3" s="83">
+      <c r="E3" s="48">
         <f t="shared" ref="E3:E4" si="0">D3/C3%</f>
         <v>0</v>
       </c>
-      <c r="F3" s="80"/>
+      <c r="F3" s="86"/>
     </row>
     <row r="4" spans="1:6" s="4" customFormat="1">
-      <c r="C4" s="79">
+      <c r="C4" s="46">
         <f>SUM(C2:C3)</f>
         <v>117</v>
       </c>
-      <c r="D4" s="79">
+      <c r="D4" s="46">
         <f>SUM(D2:D3)</f>
         <v>0</v>
       </c>
-      <c r="E4" s="84">
+      <c r="E4" s="49">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3971,6 +5096,9 @@
         <f>IF(E4&gt;=90,"APROBADO",IF(AND(E4&gt;=70,E4&lt;90),"CORREGIR","NO APROBADO"))</f>
         <v>NO APROBADO</v>
       </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="C5" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
actualizamos lista de chequeo
</commit_message>
<xml_diff>
--- a/assets/Documentación/PFPL01 - Lista de chequeo producto software (1).xlsx
+++ b/assets/Documentación/PFPL01 - Lista de chequeo producto software (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\proyectoFinal\assets\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proyectoFinal\assets\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E47BA5-592C-460D-ACBD-9BAF16CF44EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D2792A-167A-49C4-B170-9696D7466876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="930" windowWidth="20730" windowHeight="11760" tabRatio="772" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="772" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja de Control" sheetId="5" r:id="rId1"/>
@@ -31,21 +31,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="136">
   <si>
     <t>Funcionalidad</t>
   </si>
@@ -369,12 +360,6 @@
     <t>Jose bohorquez</t>
   </si>
   <si>
-    <t>el sistema (Prioridad: debe [Alta], debera [MEdia], deberia,podra [Baja], permitir)</t>
-  </si>
-  <si>
-    <t>el sistema debe permitir al administrador y empleado iniciar sesion</t>
-  </si>
-  <si>
     <t>usuarios</t>
   </si>
   <si>
@@ -451,13 +436,22 @@
   </si>
   <si>
     <t xml:space="preserve">El sistema debe permitir al administrador importar datos de productos desde un archivo CSV.	</t>
+  </si>
+  <si>
+    <t>Producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disponibilidad del sistema para proporcionar respuestas en un tiempo razonable. </t>
+  </si>
+  <si>
+    <t>garantizar que la información utilizada por cada tarea esté protegida adecuadamente contra accesos no autorizados, alteraciones o pérdidas, asegurando así la integridad y confidencialidad de los datos.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -551,6 +545,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1202,7 +1202,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1316,10 +1316,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1349,6 +1349,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1367,7 +1438,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1387,82 +1457,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel_BuiltIn_Hyperlink" xfId="2" xr:uid="{1EB9EC41-D830-4ACE-B66C-36C057A1DC02}"/>
@@ -1855,91 +1870,91 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
     </row>
     <row r="3" spans="2:6" ht="30">
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="63" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
     </row>
     <row r="4" spans="2:6" ht="30">
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
     </row>
     <row r="5" spans="2:6" ht="17.25" thickBot="1">
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
     </row>
     <row r="6" spans="2:6" ht="17.25" thickTop="1">
       <c r="F6" s="10"/>
     </row>
     <row r="8" spans="2:6" ht="30">
-      <c r="B8" s="81" t="s">
+      <c r="B8" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="81"/>
-      <c r="D8" s="81"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
     </row>
     <row r="10" spans="2:6" ht="17.25" thickBot="1"/>
     <row r="11" spans="2:6" ht="18.75" thickTop="1">
       <c r="B11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="82" t="s">
+      <c r="C11" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="83"/>
-      <c r="E11" s="83"/>
-      <c r="F11" s="84"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="61"/>
     </row>
     <row r="12" spans="2:6" ht="18">
       <c r="B12" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="68" t="s">
+      <c r="C12" s="67" t="s">
         <v>105</v>
       </c>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="70"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="69"/>
     </row>
     <row r="13" spans="2:6" ht="18.75" thickBot="1">
       <c r="B13" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="68" t="s">
+      <c r="C13" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="69"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="70"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="69"/>
     </row>
     <row r="14" spans="2:6" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="B14" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="68" t="s">
+      <c r="C14" s="67" t="s">
         <v>106</v>
       </c>
-      <c r="D14" s="72"/>
+      <c r="D14" s="71"/>
       <c r="E14" s="13" t="s">
         <v>21</v>
       </c>
@@ -1951,10 +1966,10 @@
       <c r="B15" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="73" t="s">
+      <c r="C15" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="74"/>
+      <c r="D15" s="73"/>
       <c r="E15" s="15" t="s">
         <v>25</v>
       </c>
@@ -1966,10 +1981,10 @@
       <c r="B16" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="75" t="s">
+      <c r="C16" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="76"/>
+      <c r="D16" s="75"/>
       <c r="E16" s="17" t="s">
         <v>28</v>
       </c>
@@ -1979,8 +1994,8 @@
     </row>
     <row r="17" spans="2:16" ht="17.25" thickTop="1">
       <c r="B17" s="19"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
     </row>
     <row r="18" spans="2:16" ht="19.899999999999999" customHeight="1"/>
     <row r="19" spans="2:16" ht="19.899999999999999" customHeight="1">
@@ -1999,10 +2014,10 @@
       <c r="C21" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="66" t="s">
+      <c r="D21" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="66"/>
+      <c r="E21" s="77"/>
       <c r="F21" s="24" t="s">
         <v>34</v>
       </c>
@@ -2014,10 +2029,10 @@
       <c r="C22" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="67" t="s">
+      <c r="D22" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="67"/>
+      <c r="E22" s="78"/>
       <c r="F22" s="27" t="s">
         <v>22</v>
       </c>
@@ -2025,57 +2040,57 @@
     <row r="23" spans="2:16" ht="25.5" customHeight="1">
       <c r="B23" s="28"/>
       <c r="C23" s="29"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="58"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
       <c r="F23" s="30"/>
     </row>
     <row r="24" spans="2:16" ht="25.5" customHeight="1">
       <c r="B24" s="28"/>
       <c r="C24" s="29"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="58"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="66"/>
       <c r="F24" s="30"/>
     </row>
     <row r="25" spans="2:16" ht="25.5" customHeight="1">
       <c r="B25" s="28"/>
       <c r="C25" s="29"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="66"/>
       <c r="F25" s="30"/>
     </row>
     <row r="26" spans="2:16" ht="25.5" customHeight="1">
       <c r="B26" s="28"/>
       <c r="C26" s="29"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="66"/>
       <c r="F26" s="30"/>
     </row>
     <row r="27" spans="2:16" ht="25.5" customHeight="1">
       <c r="B27" s="28"/>
       <c r="C27" s="29"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="66"/>
       <c r="F27" s="30"/>
     </row>
     <row r="28" spans="2:16" ht="25.5" customHeight="1">
       <c r="B28" s="28"/>
       <c r="C28" s="29"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="58"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
       <c r="F28" s="30"/>
     </row>
     <row r="29" spans="2:16" ht="25.5" customHeight="1">
       <c r="B29" s="28"/>
       <c r="C29" s="29"/>
-      <c r="D29" s="58"/>
-      <c r="E29" s="58"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="66"/>
       <c r="F29" s="30"/>
     </row>
     <row r="30" spans="2:16" ht="25.5" customHeight="1" thickBot="1">
       <c r="B30" s="31"/>
       <c r="C30" s="32"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="59"/>
+      <c r="D30" s="85"/>
+      <c r="E30" s="85"/>
       <c r="F30" s="33"/>
     </row>
     <row r="31" spans="2:16" ht="19.899999999999999" customHeight="1" thickTop="1"/>
@@ -2086,51 +2101,51 @@
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1" thickBot="1"/>
     <row r="34" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B34" s="60" t="s">
+      <c r="B34" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="61"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="61"/>
-      <c r="F34" s="62"/>
+      <c r="C34" s="87"/>
+      <c r="D34" s="87"/>
+      <c r="E34" s="87"/>
+      <c r="F34" s="88"/>
     </row>
     <row r="35" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B35" s="63"/>
-      <c r="C35" s="64"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="65"/>
+      <c r="B35" s="89"/>
+      <c r="C35" s="90"/>
+      <c r="D35" s="90"/>
+      <c r="E35" s="90"/>
+      <c r="F35" s="91"/>
     </row>
     <row r="36" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B36" s="52"/>
-      <c r="C36" s="53"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="54"/>
+      <c r="B36" s="79"/>
+      <c r="C36" s="80"/>
+      <c r="D36" s="80"/>
+      <c r="E36" s="80"/>
+      <c r="F36" s="81"/>
       <c r="J36" s="34" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B37" s="52"/>
-      <c r="C37" s="53"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="54"/>
+      <c r="B37" s="79"/>
+      <c r="C37" s="80"/>
+      <c r="D37" s="80"/>
+      <c r="E37" s="80"/>
+      <c r="F37" s="81"/>
     </row>
     <row r="38" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B38" s="52"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="54"/>
+      <c r="B38" s="79"/>
+      <c r="C38" s="80"/>
+      <c r="D38" s="80"/>
+      <c r="E38" s="80"/>
+      <c r="F38" s="81"/>
     </row>
     <row r="39" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B39" s="55"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="57"/>
+      <c r="B39" s="82"/>
+      <c r="C39" s="83"/>
+      <c r="D39" s="83"/>
+      <c r="E39" s="83"/>
+      <c r="F39" s="84"/>
     </row>
     <row r="40" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="A40" s="34"/>
@@ -2291,12 +2306,16 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
@@ -2309,16 +2328,12 @@
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="D25:E25"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B8:F8"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
@@ -2331,8 +2346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EC27DB5-F54D-4E92-8170-7A53853F8C0C}">
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2348,7 +2363,7 @@
         <v>46</v>
       </c>
       <c r="B1" s="43" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C1" s="41"/>
       <c r="D1" s="42"/>
@@ -2371,92 +2386,120 @@
       <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6" t="str">
-        <f>IF(C3="Cumple","Ninguna","")</f>
-        <v/>
+      <c r="B3" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="52" t="str">
+        <f>IF(C3="Cumple","Ninguna"," - El sistema debe autenticar al usuario mediante un nombre de usuario y contraseña. - El sistema debe permitir al usuario restablecer su contraseña en caso de olvido ")</f>
+        <v xml:space="preserve"> - El sistema debe autenticar al usuario mediante un nombre de usuario y contraseña. - El sistema debe permitir al usuario restablecer su contraseña en caso de olvido </v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6" t="str">
-        <f t="shared" ref="D4:D17" si="0">IF(C4="Cumple","Ninguna","")</f>
-        <v/>
+      <c r="B4" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="50" t="str">
+        <f>IF(C4="Cumple","Ninguna","- El administrador debe poder crear nuevos usuarios con diferentes roles y permisos. - El administrador debe poder editar la información de los usuarios existentes. - El administrador debe poder eliminar usuarios que ya no sean necesarios")</f>
+        <v>- El administrador debe poder crear nuevos usuarios con diferentes roles y permisos. - El administrador debe poder editar la información de los usuarios existentes. - El administrador debe poder eliminar usuarios que ya no sean necesarios</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="B5" s="50" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="50" t="str">
+        <f>IF(C5="Cumple","Ninguna","- El usuario debe poder modificar su nombre, correo electrónico y contraseña. - El usuario debe poder subir una foto de perfil")</f>
+        <v>- El usuario debe poder modificar su nombre, correo electrónico y contraseña. - El usuario debe poder subir una foto de perfil</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="B6" s="50" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" s="50" t="str">
+        <f>IF(C6="Cumple","Ninguna","- El usuario debe poder ver las acciones que ha realizado en el sistema. - El historial de actividad debe incluir la fecha, hora, acción realizada y el módulo afectado")</f>
+        <v>- El usuario debe poder ver las acciones que ha realizado en el sistema. - El historial de actividad debe incluir la fecha, hora, acción realizada y el módulo afectado</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="B7" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="50" t="str">
+        <f>IF(C7="Cumple","Ninguna","- El usuario debe poder descargar una copia de sus datos personales en un formato legible. - Los datos descargados deben incluir el nombre, correo electrónico, foto de perfil, historial de actividad y cualquier otra información personal del usuario")</f>
+        <v>- El usuario debe poder descargar una copia de sus datos personales en un formato legible. - Los datos descargados deben incluir el nombre, correo electrónico, foto de perfil, historial de actividad y cualquier otra información personal del usuario</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="B8" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="50" t="str">
+        <f>IF(C8="Cumple","Ninguna","- El usuario debe poder eliminar sus datos personales de forma permanente. - El sistema debe solicitar al usuario confirmación antes de eliminar sus datos")</f>
+        <v>- El usuario debe poder eliminar sus datos personales de forma permanente. - El sistema debe solicitar al usuario confirmación antes de eliminar sus datos</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="B9" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="50" t="str">
+        <f>IF(C9="Cumple","Ninguna","- El usuario debe poder enviar invitaciones a amigos por correo electrónico o a través de redes sociales. - Las invitaciones deben incluir un enlace para que los amigos puedan registrarse en el sistema")</f>
+        <v>- El usuario debe poder enviar invitaciones a amigos por correo electrónico o a través de redes sociales. - Las invitaciones deben incluir un enlace para que los amigos puedan registrarse en el sistema</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A10" s="8">
         <v>8</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="B10" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="50" t="str">
+        <f>IF(C10="Cumple","Ninguna","- El usuario debe poder ganar puntos o beneficios por referir amigos al sistema. - El sistema debe mostrar al usuario el número de amigos que ha referido y los puntos o beneficios que ha ganado")</f>
+        <v>- El usuario debe poder ganar puntos o beneficios por referir amigos al sistema. - El sistema debe mostrar al usuario el número de amigos que ha referido y los puntos o beneficios que ha ganado</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
@@ -2466,7 +2509,7 @@
       <c r="B11" s="6"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D4:D17" si="0">IF(C11="Cumple","Ninguna","")</f>
         <v/>
       </c>
     </row>
@@ -2540,7 +2583,9 @@
       <c r="A18" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="43"/>
+      <c r="B18" s="43" t="s">
+        <v>121</v>
+      </c>
       <c r="C18" s="41"/>
       <c r="D18" s="42"/>
     </row>
@@ -2562,44 +2607,60 @@
       <c r="A20" s="8">
         <v>16</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6" t="str">
-        <f t="shared" ref="D20:D34" si="1">IF(C20="Cumple","Ninguna","")</f>
-        <v/>
+      <c r="B20" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" s="50" t="str">
+        <f>IF(C20="Cumple","Ninguna","- El usuario debe poder seleccionar un producto y la cantidad deseada. - El sistema debe mostrar al usuario el precio total del producto, incluyendo impuestos y envío")</f>
+        <v>- El usuario debe poder seleccionar un producto y la cantidad deseada. - El sistema debe mostrar al usuario el precio total del producto, incluyendo impuestos y envío</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A21" s="8">
         <v>17</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="B21" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D21" s="50" t="str">
+        <f>IF(C21="Cumple","Ninguna","- El usuario debe poder aumentar o disminuir la cantidad de un producto en el carrito de compras. - El sistema debe actualizar automáticamente el precio total del producto")</f>
+        <v>- El usuario debe poder aumentar o disminuir la cantidad de un producto en el carrito de compras. - El sistema debe actualizar automáticamente el precio total del producto</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A22" s="8">
         <v>18</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="B22" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D22" s="50" t="str">
+        <f>IF(C22="Cumple","Ninguna","- El usuario debe poder eliminar un producto del carrito de compras. - El sistema debe actualizar automáticamente el precio total del carrito de compras")</f>
+        <v>- El usuario debe poder eliminar un producto del carrito de compras. - El sistema debe actualizar automáticamente el precio total del carrito de compras</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A23" s="8">
         <v>19</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="B23" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="50" t="str">
+        <f>IF(C23="Cumple","Ninguna","- El usuario debe poder seleccionar un método de pago, como tarjeta de crédito, débito o PayPal. - El sistema debe procesar el pago de forma segura y enviar un correo electrónico de confirmación al usuario")</f>
+        <v>- El usuario debe poder seleccionar un método de pago, como tarjeta de crédito, débito o PayPal. - El sistema debe procesar el pago de forma segura y enviar un correo electrónico de confirmación al usuario</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
@@ -2609,7 +2670,7 @@
       <c r="B24" s="6"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D20:D34" si="1">IF(C24="Cumple","Ninguna","")</f>
         <v/>
       </c>
     </row>
@@ -2727,7 +2788,9 @@
       <c r="A35" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="43"/>
+      <c r="B35" s="43" t="s">
+        <v>133</v>
+      </c>
       <c r="C35" s="41"/>
       <c r="D35" s="42"/>
     </row>
@@ -2749,110 +2812,150 @@
       <c r="A37" s="8">
         <v>31</v>
       </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="6" t="str">
-        <f t="shared" ref="D37:D51" si="2">IF(C37="Cumple","Ninguna","")</f>
-        <v/>
+      <c r="B37" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" s="50" t="str">
+        <f>IF(C37="Cumple","Ninguna","- El sistema debe mostrar al usuario una lista de productos con imágenes, nombre, precio y descripción")</f>
+        <v>- El sistema debe mostrar al usuario una lista de productos con imágenes, nombre, precio y descripción</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A38" s="8">
         <v>32</v>
       </c>
-      <c r="B38" s="6"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="B38" s="50" t="s">
+        <v>124</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="50" t="str">
+        <f>IF(C38="Cumple","Ninguna","- El usuario debe poder ver los detalles de un producto específico, incluyendo imágenes, descripción, precio, disponibilidad, características y especificaciones")</f>
+        <v>- El usuario debe poder ver los detalles de un producto específico, incluyendo imágenes, descripción, precio, disponibilidad, características y especificaciones</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A39" s="8">
         <v>33</v>
       </c>
-      <c r="B39" s="6"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="B39" s="50" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" s="50" t="str">
+        <f>IF(C39="Cumple","Ninguna","- El administrador debe poder establecer el precio, la disponibilidad, las características y las especificaciones de un producto. - El administrador debe poder subir imágenes del producto")</f>
+        <v>- El administrador debe poder establecer el precio, la disponibilidad, las características y las especificaciones de un producto. - El administrador debe poder subir imágenes del producto</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A40" s="8">
         <v>34</v>
       </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="B40" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D40" s="50" t="str">
+        <f>IF(C40="Cumple","Ninguna","- El usuario debe poder editar la cantidad de un producto en el carrito de compras. - El usuario debe poder eliminar un producto del carrito de compras")</f>
+        <v>- El usuario debe poder editar la cantidad de un producto en el carrito de compras. - El usuario debe poder eliminar un producto del carrito de compras</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A41" s="8">
         <v>35</v>
       </c>
-      <c r="B41" s="6"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="B41" s="50" t="s">
+        <v>127</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D41" s="50" t="str">
+        <f>IF(C41="Cumple","Ninguna","- El sistema debe aceptar diferentes métodos de pago, como tarjeta de crédito, débito o PayPal. - El sistema debe procesar el pago de forma segura y enviar un correo electrónico de confirmación al usuario")</f>
+        <v>- El sistema debe aceptar diferentes métodos de pago, como tarjeta de crédito, débito o PayPal. - El sistema debe procesar el pago de forma segura y enviar un correo electrónico de confirmación al usuario</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A42" s="8">
         <v>36</v>
       </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="B42" s="50" t="s">
+        <v>128</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" s="50" t="str">
+        <f>IF(C42="Cumple","Ninguna","- El usuario debe poder ver el estado de su pedido. - El sistema debe enviar un correo electrónico de confirmación al usuario cuando se envíe su pedido")</f>
+        <v>- El usuario debe poder ver el estado de su pedido. - El sistema debe enviar un correo electrónico de confirmación al usuario cuando se envíe su pedido</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A43" s="8">
         <v>37</v>
       </c>
-      <c r="B43" s="6"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="B43" s="50" t="s">
+        <v>129</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43" s="50" t="str">
+        <f>IF(C43="Cumple","Ninguna","- El usuario debe poder ver los detalles de cada compra, como la fecha, el número de pedido, los productos comprados y el precio total")</f>
+        <v>- El usuario debe poder ver los detalles de cada compra, como la fecha, el número de pedido, los productos comprados y el precio total</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A44" s="8">
         <v>38</v>
       </c>
-      <c r="B44" s="6"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="B44" s="50" t="s">
+        <v>130</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D44" s="50" t="str">
+        <f>IF(C44="Cumple","Ninguna","- El sistema debe mostrar las calificaciones y reseñas de los productos a otros usuarios")</f>
+        <v>- El sistema debe mostrar las calificaciones y reseñas de los productos a otros usuarios</v>
       </c>
     </row>
     <row r="45" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A45" s="8">
         <v>39</v>
       </c>
-      <c r="B45" s="6"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="B45" s="50" t="s">
+        <v>131</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D45" s="50" t="str">
+        <f>IF(C45="Cumple","Ninguna","- El sistema debe mantener un registro del inventario de productos. - El sistema debe alertar al administrador cuando el inventario de un producto esté bajo")</f>
+        <v>- El sistema debe mantener un registro del inventario de productos. - El sistema debe alertar al administrador cuando el inventario de un producto esté bajo</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A46" s="8">
         <v>40</v>
       </c>
-      <c r="B46" s="6"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="B46" s="50" t="s">
+        <v>132</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" s="50" t="str">
+        <f>IF(C46="Cumple","Ninguna","- El sistema debe permitir al administrador exportar datos de productos a un archivo CSV")</f>
+        <v>- El sistema debe permitir al administrador exportar datos de productos a un archivo CSV</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
@@ -2862,7 +2965,7 @@
       <c r="B47" s="6"/>
       <c r="C47" s="5"/>
       <c r="D47" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D37:D51" si="2">IF(C47="Cumple","Ninguna","")</f>
         <v/>
       </c>
     </row>
@@ -2894,7 +2997,7 @@
       </c>
       <c r="B50" s="6"/>
       <c r="C50" s="5"/>
-      <c r="D50" s="6" t="str">
+      <c r="D50" s="94" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3121,7 +3224,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C17 C20:C34 C37:C51 C54:C68" xr:uid="{F381E73E-C892-4E35-A1B1-7DCF65F35B27}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C54:C68 C3:C17 C20:C34 C37:C51" xr:uid="{F381E73E-C892-4E35-A1B1-7DCF65F35B27}">
       <formula1>"Cumple, No Cumple"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3133,39 +3236,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E8C143B-B431-458E-8866-1207E50001AB}">
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.42578125" style="90" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.42578125" style="55" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="77.5703125" style="90" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77.5703125" style="55" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A1" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="91" t="s">
-        <v>109</v>
+      <c r="B1" s="56" t="s">
+        <v>107</v>
       </c>
       <c r="C1" s="41"/>
-      <c r="D1" s="88"/>
+      <c r="D1" s="53"/>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="54" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="89" t="s">
+      <c r="D2" s="54" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3174,12 +3277,12 @@
         <v>1</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" s="87" t="str">
+        <v>113</v>
+      </c>
+      <c r="D3" s="52" t="str">
         <f>IF(C3="Cumple","Ninguna"," - El sistema debe autenticar al usuario mediante un nombre de usuario y contraseña. - El sistema debe permitir al usuario restablecer su contraseña en caso de olvido ")</f>
         <v xml:space="preserve"> - El sistema debe autenticar al usuario mediante un nombre de usuario y contraseña. - El sistema debe permitir al usuario restablecer su contraseña en caso de olvido </v>
       </c>
@@ -3189,10 +3292,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D4" s="50" t="str">
         <f>IF(C4="Cumple","Ninguna","- El administrador debe poder crear nuevos usuarios con diferentes roles y permisos. - El administrador debe poder editar la información de los usuarios existentes. - El administrador debe poder eliminar usuarios que ya no sean necesarios")</f>
@@ -3204,10 +3307,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D5" s="50" t="str">
         <f>IF(C5="Cumple","Ninguna","- El usuario debe poder modificar su nombre, correo electrónico y contraseña. - El usuario debe poder subir una foto de perfil")</f>
@@ -3219,10 +3322,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D6" s="50" t="str">
         <f>IF(C6="Cumple","Ninguna","- El usuario debe poder ver las acciones que ha realizado en el sistema. - El historial de actividad debe incluir la fecha, hora, acción realizada y el módulo afectado")</f>
@@ -3234,10 +3337,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D7" s="50" t="str">
         <f>IF(C7="Cumple","Ninguna","- El usuario debe poder descargar una copia de sus datos personales en un formato legible. - Los datos descargados deben incluir el nombre, correo electrónico, foto de perfil, historial de actividad y cualquier otra información personal del usuario")</f>
@@ -3249,10 +3352,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D8" s="50" t="str">
         <f>IF(C8="Cumple","Ninguna","- El usuario debe poder eliminar sus datos personales de forma permanente. - El sistema debe solicitar al usuario confirmación antes de eliminar sus datos")</f>
@@ -3264,10 +3367,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D9" s="50" t="str">
         <f>IF(C9="Cumple","Ninguna","- El usuario debe poder enviar invitaciones a amigos por correo electrónico o a través de redes sociales. - Las invitaciones deben incluir un enlace para que los amigos puedan registrarse en el sistema")</f>
@@ -3279,10 +3382,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D10" s="50" t="str">
         <f>IF(C10="Cumple","Ninguna","- El usuario debe poder ganar puntos o beneficios por referir amigos al sistema. - El sistema debe mostrar al usuario el número de amigos que ha referido y los puntos o beneficios que ha ganado")</f>
@@ -3328,7 +3431,7 @@
       <c r="B15" s="50"/>
       <c r="C15" s="5"/>
       <c r="D15" s="50" t="str">
-        <f t="shared" ref="D4:D17" si="0">IF(C15="Cumple","Ninguna","")</f>
+        <f t="shared" ref="D15:D17" si="0">IF(C15="Cumple","Ninguna","")</f>
         <v/>
       </c>
     </row>
@@ -3358,23 +3461,23 @@
       <c r="A18" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="91" t="s">
-        <v>123</v>
+      <c r="B18" s="56" t="s">
+        <v>121</v>
       </c>
       <c r="C18" s="41"/>
-      <c r="D18" s="88"/>
+      <c r="D18" s="53"/>
     </row>
     <row r="19" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A19" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="89" t="s">
+      <c r="B19" s="54" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="89" t="s">
+      <c r="D19" s="54" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3383,10 +3486,10 @@
         <v>16</v>
       </c>
       <c r="B20" s="50" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D20" s="50" t="str">
         <f>IF(C20="Cumple","Ninguna","- El usuario debe poder seleccionar un producto y la cantidad deseada. - El sistema debe mostrar al usuario el precio total del producto, incluyendo impuestos y envío")</f>
@@ -3398,10 +3501,10 @@
         <v>17</v>
       </c>
       <c r="B21" s="50" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D21" s="50" t="str">
         <f>IF(C21="Cumple","Ninguna","- El usuario debe poder aumentar o disminuir la cantidad de un producto en el carrito de compras. - El sistema debe actualizar automáticamente el precio total del producto")</f>
@@ -3413,10 +3516,10 @@
         <v>18</v>
       </c>
       <c r="B22" s="50" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D22" s="50" t="str">
         <f>IF(C22="Cumple","Ninguna","- El usuario debe poder eliminar un producto del carrito de compras. - El sistema debe actualizar automáticamente el precio total del carrito de compras")</f>
@@ -3428,10 +3531,10 @@
         <v>19</v>
       </c>
       <c r="B23" s="50" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D23" s="50" t="str">
         <f>IF(C23="Cumple","Ninguna","- El usuario debe poder seleccionar un método de pago, como tarjeta de crédito, débito o PayPal. - El sistema debe procesar el pago de forma segura y enviar un correo electrónico de confirmación al usuario")</f>
@@ -3445,7 +3548,7 @@
       <c r="B24" s="50"/>
       <c r="C24" s="5"/>
       <c r="D24" s="50" t="str">
-        <f t="shared" ref="D20:D34" si="1">IF(C24="Cumple","Ninguna","")</f>
+        <f t="shared" ref="D24:D34" si="1">IF(C24="Cumple","Ninguna","")</f>
         <v/>
       </c>
     </row>
@@ -3563,23 +3666,23 @@
       <c r="A35" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="91" t="s">
-        <v>124</v>
+      <c r="B35" s="56" t="s">
+        <v>122</v>
       </c>
       <c r="C35" s="41"/>
-      <c r="D35" s="88"/>
+      <c r="D35" s="53"/>
     </row>
     <row r="36" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A36" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="89" t="s">
+      <c r="B36" s="54" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="89" t="s">
+      <c r="D36" s="54" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3588,10 +3691,10 @@
         <v>31</v>
       </c>
       <c r="B37" s="50" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D37" s="50" t="str">
         <f>IF(C37="Cumple","Ninguna","- El sistema debe mostrar al usuario una lista de productos con imágenes, nombre, precio y descripción")</f>
@@ -3603,10 +3706,10 @@
         <v>32</v>
       </c>
       <c r="B38" s="50" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D38" s="50" t="str">
         <f>IF(C38="Cumple","Ninguna","- El usuario debe poder ver los detalles de un producto específico, incluyendo imágenes, descripción, precio, disponibilidad, características y especificaciones")</f>
@@ -3618,10 +3721,10 @@
         <v>33</v>
       </c>
       <c r="B39" s="50" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D39" s="50" t="str">
         <f>IF(C39="Cumple","Ninguna","- El administrador debe poder establecer el precio, la disponibilidad, las características y las especificaciones de un producto. - El administrador debe poder subir imágenes del producto")</f>
@@ -3633,10 +3736,10 @@
         <v>34</v>
       </c>
       <c r="B40" s="50" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D40" s="50" t="str">
         <f>IF(C40="Cumple","Ninguna","- El usuario debe poder editar la cantidad de un producto en el carrito de compras. - El usuario debe poder eliminar un producto del carrito de compras")</f>
@@ -3648,10 +3751,10 @@
         <v>35</v>
       </c>
       <c r="B41" s="50" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D41" s="50" t="str">
         <f>IF(C41="Cumple","Ninguna","- El sistema debe aceptar diferentes métodos de pago, como tarjeta de crédito, débito o PayPal. - El sistema debe procesar el pago de forma segura y enviar un correo electrónico de confirmación al usuario")</f>
@@ -3663,10 +3766,10 @@
         <v>36</v>
       </c>
       <c r="B42" s="50" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D42" s="50" t="str">
         <f>IF(C42="Cumple","Ninguna","- El usuario debe poder ver el estado de su pedido. - El sistema debe enviar un correo electrónico de confirmación al usuario cuando se envíe su pedido")</f>
@@ -3678,10 +3781,10 @@
         <v>37</v>
       </c>
       <c r="B43" s="50" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D43" s="50" t="str">
         <f>IF(C43="Cumple","Ninguna","- El usuario debe poder ver los detalles de cada compra, como la fecha, el número de pedido, los productos comprados y el precio total")</f>
@@ -3693,10 +3796,10 @@
         <v>38</v>
       </c>
       <c r="B44" s="50" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D44" s="50" t="str">
         <f>IF(C44="Cumple","Ninguna","- El sistema debe mostrar las calificaciones y reseñas de los productos a otros usuarios")</f>
@@ -3708,10 +3811,10 @@
         <v>39</v>
       </c>
       <c r="B45" s="50" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D45" s="50" t="str">
         <f>IF(C45="Cumple","Ninguna","- El sistema debe mantener un registro del inventario de productos. - El sistema debe alertar al administrador cuando el inventario de un producto esté bajo")</f>
@@ -3723,10 +3826,10 @@
         <v>40</v>
       </c>
       <c r="B46" s="50" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D46" s="50" t="str">
         <f>IF(C46="Cumple","Ninguna","- El sistema debe permitir al administrador exportar datos de productos a un archivo CSV")</f>
@@ -3739,8 +3842,8 @@
       </c>
       <c r="B47" s="50"/>
       <c r="C47" s="5"/>
-      <c r="D47" s="50" t="str">
-        <f t="shared" ref="D37:D51" si="2">IF(C47="Cumple","Ninguna","")</f>
+      <c r="D47" s="98" t="str">
+        <f t="shared" ref="D47:D51" si="2">IF(C47="Cumple","Ninguna","")</f>
         <v/>
       </c>
     </row>
@@ -3792,21 +3895,21 @@
       <c r="A52" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="B52" s="91"/>
+      <c r="B52" s="56"/>
       <c r="C52" s="41"/>
-      <c r="D52" s="88"/>
+      <c r="D52" s="53"/>
     </row>
     <row r="53" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A53" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B53" s="89" t="s">
+      <c r="B53" s="54" t="s">
         <v>5</v>
       </c>
       <c r="C53" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="89" t="s">
+      <c r="D53" s="54" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3979,21 +4082,21 @@
       <c r="A69" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="B69" s="91"/>
+      <c r="B69" s="56"/>
       <c r="C69" s="41"/>
-      <c r="D69" s="88"/>
+      <c r="D69" s="53"/>
     </row>
     <row r="70" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A70" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B70" s="89" t="s">
+      <c r="B70" s="54" t="s">
         <v>5</v>
       </c>
       <c r="C70" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D70" s="89" t="s">
+      <c r="D70" s="54" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4012,8 +4115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4021,7 +4124,7 @@
     <col min="1" max="1" width="12.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="90.7109375" style="51" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="70.7109375" customWidth="1"/>
+    <col min="4" max="4" width="83.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
@@ -4042,30 +4145,28 @@
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="92" t="s">
-        <v>115</v>
-      </c>
-      <c r="D2" s="6" t="str">
-        <f>IF(C2="Cumple","Ninguna","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
+      <c r="C2" s="57" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="95" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="4" customFormat="1" ht="51.75">
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="97" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" s="6" t="str">
-        <f t="shared" ref="D3:D65" si="0">IF(C3="Cumple","Ninguna","")</f>
-        <v/>
+        <v>113</v>
+      </c>
+      <c r="D3" s="96" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
@@ -4076,10 +4177,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D4" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D3:D65" si="0">IF(C4="Cumple","Ninguna","")</f>
         <v/>
       </c>
     </row>
@@ -4091,7 +4192,7 @@
         <v>51</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4106,7 +4207,7 @@
         <v>52</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4121,7 +4222,7 @@
         <v>53</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4136,7 +4237,7 @@
         <v>54</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4151,7 +4252,7 @@
         <v>55</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4180,7 +4281,7 @@
         <v>56</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4195,7 +4296,7 @@
         <v>57</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4210,7 +4311,7 @@
         <v>58</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4225,7 +4326,7 @@
         <v>59</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4240,7 +4341,7 @@
         <v>61</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4255,7 +4356,7 @@
         <v>60</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4270,7 +4371,7 @@
         <v>62</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4299,7 +4400,7 @@
         <v>63</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4314,7 +4415,7 @@
         <v>64</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4329,7 +4430,7 @@
         <v>65</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4344,7 +4445,7 @@
         <v>66</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4359,7 +4460,7 @@
         <v>67</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4374,7 +4475,7 @@
         <v>68</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4389,7 +4490,7 @@
         <v>69</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4404,7 +4505,7 @@
         <v>70</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4433,7 +4534,7 @@
         <v>71</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4448,7 +4549,7 @@
         <v>72</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4463,7 +4564,7 @@
         <v>73</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4478,7 +4579,7 @@
         <v>74</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4493,7 +4594,7 @@
         <v>75</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4508,7 +4609,7 @@
         <v>76</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D33" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4537,7 +4638,7 @@
         <v>77</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4552,7 +4653,7 @@
         <v>78</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4567,7 +4668,7 @@
         <v>79</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4596,7 +4697,7 @@
         <v>80</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4611,7 +4712,7 @@
         <v>81</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4626,7 +4727,7 @@
         <v>82</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D41" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4641,7 +4742,7 @@
         <v>83</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D42" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4656,7 +4757,7 @@
         <v>84</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D43" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4671,7 +4772,7 @@
         <v>85</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D44" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4686,7 +4787,7 @@
         <v>86</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D45" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4701,7 +4802,7 @@
         <v>87</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D46" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4716,7 +4817,7 @@
         <v>88</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D47" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4731,7 +4832,7 @@
         <v>89</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D48" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4760,7 +4861,7 @@
         <v>90</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D50" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4775,7 +4876,7 @@
         <v>91</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D51" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4790,7 +4891,7 @@
         <v>92</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D52" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4805,7 +4906,7 @@
         <v>93</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D53" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4820,7 +4921,7 @@
         <v>94</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D54" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4835,7 +4936,7 @@
         <v>95</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D55" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4850,7 +4951,7 @@
         <v>96</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D56" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4865,7 +4966,7 @@
         <v>97</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D57" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4880,7 +4981,7 @@
         <v>98</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D58" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4895,7 +4996,7 @@
         <v>99</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D59" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4924,7 +5025,7 @@
         <v>100</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D61" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4939,7 +5040,7 @@
         <v>101</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D62" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4954,7 +5055,7 @@
         <v>102</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D63" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4969,7 +5070,7 @@
         <v>103</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D64" s="6" t="str">
         <f t="shared" si="0"/>
@@ -4984,7 +5085,7 @@
         <v>104</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D65" s="6" t="str">
         <f t="shared" si="0"/>
@@ -5005,7 +5106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D51D51-DE4C-4B5C-90F6-8EADB68EB458}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+    <sheetView zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -5033,7 +5134,7 @@
       <c r="E1" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="85" t="s">
+      <c r="F1" s="92" t="s">
         <v>49</v>
       </c>
     </row>
@@ -5056,7 +5157,7 @@
         <f>D2/C2%</f>
         <v>0</v>
       </c>
-      <c r="F2" s="86"/>
+      <c r="F2" s="93"/>
     </row>
     <row r="3" spans="1:6" s="4" customFormat="1">
       <c r="A3" s="47">
@@ -5077,7 +5178,7 @@
         <f t="shared" ref="E3:E4" si="0">D3/C3%</f>
         <v>0</v>
       </c>
-      <c r="F3" s="86"/>
+      <c r="F3" s="93"/>
     </row>
     <row r="4" spans="1:6" s="4" customFormat="1">
       <c r="C4" s="46">
@@ -5098,7 +5199,7 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="C5" s="93"/>
+      <c r="C5" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>